<commit_message>
2.5.0 add variable name
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CE1B8B-A5DC-4AAC-8EA9-8A43D2C5A0D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122F0880-A3C8-4A97-8858-BB1D6CB74DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="5115" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_map" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -160,9 +160,6 @@
     <t>is_boss</t>
   </si>
   <si>
-    <t>testfloat</t>
-  </si>
-  <si>
     <t>teststring</t>
   </si>
   <si>
@@ -214,7 +211,16 @@
     <t>{"IsStringId":false,"IsGenItemClass":false,"JSONName":"st_mapJSON"}</t>
   </si>
   <si>
-    <t>{"IsStringId":false,"IsGenItemClass":false,"JSONName":"st_levelJSON"}</t>
+    <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_levelJSON"}</t>
+  </si>
+  <si>
+    <t>float:row</t>
+  </si>
+  <si>
+    <t>string:col</t>
+  </si>
+  <si>
+    <t>bool:testfloat</t>
   </si>
 </sst>
 </file>
@@ -627,7 +633,7 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -729,7 +735,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,7 +748,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" t="s">
         <v>10</v>
@@ -753,10 +759,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -771,16 +777,16 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
       <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
         <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -809,13 +815,13 @@
         <v>2.5</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -835,13 +841,13 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
         <v>24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -861,13 +867,13 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" t="s">
         <v>26</v>
-      </c>
-      <c r="K5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -893,13 +899,13 @@
         <v>2.4</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" t="s">
         <v>28</v>
-      </c>
-      <c r="K6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -919,13 +925,13 @@
         <v>1.2</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="s">
         <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
3.1.1 support save enum to json file
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF9031B-8C70-4848-98C6-70C8D44DA6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13C5F6A-578A-4128-9AAD-7962088FE698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5115" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>id</t>
   </si>
@@ -238,10 +238,13 @@
     <t>{"IsStringId":false,"IsGenItemClass":false,"JSONName":"st_mapJSON","IsGenEnum":false}</t>
   </si>
   <si>
-    <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_levelJSON","IsGenEnum":false}</t>
-  </si>
-  <si>
-    <t>Resources/subFolder</t>
+    <t>ENUM1:5</t>
+  </si>
+  <si>
+    <t>ENUM3:67</t>
+  </si>
+  <si>
+    <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_levelJSON","IsGenEnum":true,"Path":"toanstt"}</t>
   </si>
 </sst>
 </file>
@@ -758,10 +761,13 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="A1:O7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -771,10 +777,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -859,10 +862,10 @@
         <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="N3" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
can select skip to generate any enum
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41006C28-B609-4E0C-ABA5-2DD580A95150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3039F34-80CF-4D52-8E5E-C9EABEF90E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5625" yWindow="2730" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="47">
   <si>
     <t>id</t>
   </si>
@@ -1041,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA2FB3B-55EE-4F82-BAA9-C5D77386B2AC}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:O7"/>
+      <selection activeCell="F14" sqref="A11:O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,6 +1288,245 @@
         <v>35</v>
       </c>
     </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>23</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>2.5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14" t="s">
+        <v>36</v>
+      </c>
+      <c r="N14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" t="s">
+        <v>36</v>
+      </c>
+      <c r="M15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>2.4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
+        <v>26</v>
+      </c>
+      <c r="K16" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>1.2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L17" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add warning if array have empty cells in middle
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7017F8-E4CF-477D-AC21-B418D61C88F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BF54FB-A3A9-4D11-BEA1-B8207E038DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="2430" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6750" yWindow="2775" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_map" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="48">
   <si>
     <t>id</t>
   </si>
@@ -1047,7 +1047,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1340,7 +1340,7 @@
         <v>33</v>
       </c>
       <c r="M12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N12" t="s">
         <v>38</v>
@@ -1457,6 +1457,9 @@
         <v>36</v>
       </c>
       <c r="M15" t="s">
+        <v>36</v>
+      </c>
+      <c r="N15" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bug gen id
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BF54FB-A3A9-4D11-BEA1-B8207E038DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA4FDAF-3001-49F3-AB01-046B61C4B7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6750" yWindow="2775" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-1800" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_map" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="50">
   <si>
     <t>id</t>
   </si>
@@ -258,6 +258,12 @@
   </si>
   <si>
     <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_levelJSON","IsGenEnum":true,"Path":"toanstt/Resources/toandata","IsSeparatedJSON":true}</t>
+  </si>
+  <si>
+    <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_levelJSON","IsGenEnum":true,"Path":"toanstt","IsSeparatedJSON":true}</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -1047,7 +1053,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,12 +1305,12 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
add GetAllIds() function for separated JSON files
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B150CDD7-39D3-4144-8C76-A705192F44BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BC0988-55D8-4484-B51A-E9841649EC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="3015" windowWidth="16410" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_map" sheetId="1" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -264,6 +264,21 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>r4r</t>
+  </si>
+  <si>
+    <t>5r4</t>
+  </si>
+  <si>
+    <t>ffd</t>
+  </si>
+  <si>
+    <t>45fe</t>
+  </si>
+  <si>
+    <t>34f</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA2FB3B-55EE-4F82-BAA9-C5D77386B2AC}">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1486,7 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16">
         <v>4</v>
@@ -1507,7 +1522,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1536,6 +1551,248 @@
         <v>35</v>
       </c>
       <c r="M17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" t="s">
+        <v>33</v>
+      </c>
+      <c r="M23" t="s">
+        <v>37</v>
+      </c>
+      <c r="N23" t="s">
+        <v>38</v>
+      </c>
+      <c r="O23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>23</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>2.5</v>
+      </c>
+      <c r="I24" t="s">
+        <v>15</v>
+      </c>
+      <c r="J24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" t="s">
+        <v>41</v>
+      </c>
+      <c r="M24" t="s">
+        <v>42</v>
+      </c>
+      <c r="N24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>15</v>
+      </c>
+      <c r="J25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" t="s">
+        <v>23</v>
+      </c>
+      <c r="L25" t="s">
+        <v>36</v>
+      </c>
+      <c r="M25" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="I26" t="s">
+        <v>15</v>
+      </c>
+      <c r="J26" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" t="s">
+        <v>36</v>
+      </c>
+      <c r="M26" t="s">
+        <v>36</v>
+      </c>
+      <c r="N26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="H27">
+        <v>2.4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>16</v>
+      </c>
+      <c r="J27" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L27" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28">
+        <v>4</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>1.2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>17</v>
+      </c>
+      <c r="J28" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" t="s">
+        <v>29</v>
+      </c>
+      <c r="L28" t="s">
+        <v>35</v>
+      </c>
+      <c r="M28" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
support fast define enum
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEA9DA0-7B6E-4F87-96EB-A45B9A596A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2519D4A-18F9-4D6A-8EA2-16460C0A6E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9000" yWindow="3015" windowWidth="24840" windowHeight="15345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_map" sheetId="1" r:id="rId1"/>
     <sheet name="st_level" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -282,6 +283,30 @@
   </si>
   <si>
     <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_levelJSON","IsGenEnum":true,"Path":"toanstt","IsSeparatedJSON":false}</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>myenum{A,B,C}:nameenum</t>
+  </si>
+  <si>
+    <t>my:name</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>D 4</t>
+  </si>
+  <si>
+    <t>myenum{A 0,B 14,C 23}:nameenum</t>
   </si>
 </sst>
 </file>
@@ -1068,15 +1093,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA2FB3B-55EE-4F82-BAA9-C5D77386B2AC}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="A11:O17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="A1:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1087,7 +1112,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1133,8 +1158,11 @@
       <c r="O2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1177,8 +1205,11 @@
       <c r="N3" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1212,8 +1243,11 @@
       <c r="N4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1244,8 +1278,11 @@
       <c r="M5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1282,8 +1319,11 @@
       <c r="M6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1314,8 +1354,11 @@
       <c r="M7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1326,7 +1369,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1373,7 +1416,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1417,7 +1460,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1452,7 +1495,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1487,7 +1530,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1798,6 +1841,106 @@
       <c r="M28" t="s">
         <v>35</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA569B3A-36DC-4A9C-8790-9E179146205E}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
move type to right part
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2519D4A-18F9-4D6A-8EA2-16460C0A6E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5AA05D-54F4-48D6-A088-596E063DBA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9000" yWindow="3015" windowWidth="24840" windowHeight="15345" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9195" yWindow="4050" windowWidth="20445" windowHeight="15345" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_map" sheetId="1" r:id="rId1"/>
     <sheet name="st_level" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -115,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="101">
   <si>
     <t>id</t>
   </si>
@@ -207,18 +208,6 @@
     <t>strings6</t>
   </si>
   <si>
-    <t>float:row</t>
-  </si>
-  <si>
-    <t>string:col</t>
-  </si>
-  <si>
-    <t>bool:testfloat</t>
-  </si>
-  <si>
-    <t>TestEnum:testenum</t>
-  </si>
-  <si>
     <t>ENUM1</t>
   </si>
   <si>
@@ -228,18 +217,6 @@
     <t>ENUM2</t>
   </si>
   <si>
-    <t>TestEnum:e0</t>
-  </si>
-  <si>
-    <t>TestEnum:e1</t>
-  </si>
-  <si>
-    <t>TestEnum:e2</t>
-  </si>
-  <si>
-    <t>{"IsStringId":false,"IsGenItemClass":false,"JSONName":"st_mapJSON","IsGenEnum":false}</t>
-  </si>
-  <si>
     <t>ENUM1:5</t>
   </si>
   <si>
@@ -249,15 +226,6 @@
     <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_levelJSON","IsGenEnum":true,"Path":"toanstt"}</t>
   </si>
   <si>
-    <t>TestEnum{true}:e0</t>
-  </si>
-  <si>
-    <t>TestEnum{true}:e1</t>
-  </si>
-  <si>
-    <t>TestEnum{true}:e2</t>
-  </si>
-  <si>
     <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_levelJSON","IsGenEnum":true,"Path":"toanstt/Resources/toandata","IsSeparatedJSON":true}</t>
   </si>
   <si>
@@ -288,9 +256,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>myenum{A,B,C}:nameenum</t>
-  </si>
-  <si>
     <t>my:name</t>
   </si>
   <si>
@@ -303,10 +268,157 @@
     <t>F</t>
   </si>
   <si>
-    <t>D 4</t>
-  </si>
-  <si>
-    <t>myenum{A 0,B 14,C 23}:nameenum</t>
+    <t>StEnemy</t>
+  </si>
+  <si>
+    <t>StEnemyTable</t>
+  </si>
+  <si>
+    <t>{}</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Prefab</t>
+  </si>
+  <si>
+    <t>shootableRange0:Float</t>
+  </si>
+  <si>
+    <t>ShootInterval0:Float</t>
+  </si>
+  <si>
+    <t>ShootCount0:Float</t>
+  </si>
+  <si>
+    <t>BulletInterval0:Float</t>
+  </si>
+  <si>
+    <t>BulletPrefab</t>
+  </si>
+  <si>
+    <t>Damage</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>HealthBarSizeX</t>
+  </si>
+  <si>
+    <t>HealthBarSizeY</t>
+  </si>
+  <si>
+    <t>HealthBarDY</t>
+  </si>
+  <si>
+    <t>fx_die</t>
+  </si>
+  <si>
+    <t>Soldier</t>
+  </si>
+  <si>
+    <t>EenemySoldier</t>
+  </si>
+  <si>
+    <t>20.1,28</t>
+  </si>
+  <si>
+    <t>1.5,2</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>0.2,0.3</t>
+  </si>
+  <si>
+    <t>BulletSoldier</t>
+  </si>
+  <si>
+    <t>Soul</t>
+  </si>
+  <si>
+    <t>LandingCraft</t>
+  </si>
+  <si>
+    <t>EnemyLandingCraft</t>
+  </si>
+  <si>
+    <t>NukeConeExplosionFire</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>EnemyTank</t>
+  </si>
+  <si>
+    <t>30.1,40</t>
+  </si>
+  <si>
+    <t>2.5,3</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>BulletTank</t>
+  </si>
+  <si>
+    <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_mapJSON","IsGenEnum":false}</t>
+  </si>
+  <si>
+    <t>row:float</t>
+  </si>
+  <si>
+    <t>col:string</t>
+  </si>
+  <si>
+    <t>testfloat:float</t>
+  </si>
+  <si>
+    <t>testenum:TestEnum</t>
+  </si>
+  <si>
+    <t>e1</t>
+  </si>
+  <si>
+    <t>e2</t>
+  </si>
+  <si>
+    <t>e3</t>
+  </si>
+  <si>
+    <t>ENUM2:234</t>
+  </si>
+  <si>
+    <t>ENUM7:322</t>
+  </si>
+  <si>
+    <t>e0:TestEnum</t>
+  </si>
+  <si>
+    <t>ENUM8</t>
+  </si>
+  <si>
+    <t>testfloat:bool</t>
+  </si>
+  <si>
+    <t>e0:TestEnum{true}</t>
+  </si>
+  <si>
+    <t>nameenum1</t>
+  </si>
+  <si>
+    <t>nameenum0:PENUM2{B,C,D 55,R}</t>
+  </si>
+  <si>
+    <t>D:4</t>
+  </si>
+  <si>
+    <t>nameenum:Kmyenum{A 0,B 14,C 23}</t>
   </si>
 </sst>
 </file>
@@ -361,9 +473,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -705,7 +818,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C3" sqref="A1:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +834,7 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>40</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -823,7 +936,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:O7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -839,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -847,10 +960,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -865,7 +978,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
@@ -877,16 +990,16 @@
         <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="M2" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="O2" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -924,13 +1037,16 @@
         <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -959,13 +1075,16 @@
         <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -994,10 +1113,10 @@
         <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="M5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1032,10 +1151,10 @@
         <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1064,10 +1183,10 @@
         <v>29</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
@@ -1093,15 +1212,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA2FB3B-55EE-4F82-BAA9-C5D77386B2AC}">
-  <dimension ref="A1:P28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="A1:P7"/>
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1109,18 +1228,18 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -1135,7 +1254,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
@@ -1147,22 +1266,25 @@
         <v>19</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="M2" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="O2" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="P2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1197,19 +1319,19 @@
         <v>21</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1235,19 +1357,19 @@
         <v>23</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="P4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1273,16 +1395,16 @@
         <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="P5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1314,16 +1436,16 @@
         <v>27</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1349,16 +1471,16 @@
         <v>29</v>
       </c>
       <c r="L7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="P7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1366,18 +1488,18 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
@@ -1392,7 +1514,7 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
@@ -1404,19 +1526,19 @@
         <v>19</v>
       </c>
       <c r="L12" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="M12" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="N12" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="O12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1451,16 +1573,16 @@
         <v>21</v>
       </c>
       <c r="L13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="M13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1486,16 +1608,16 @@
         <v>23</v>
       </c>
       <c r="L14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1521,16 +1643,16 @@
         <v>25</v>
       </c>
       <c r="L15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1562,10 +1684,10 @@
         <v>27</v>
       </c>
       <c r="L16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1594,10 +1716,10 @@
         <v>29</v>
       </c>
       <c r="L17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -1608,18 +1730,18 @@
         <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
         <v>13</v>
@@ -1634,7 +1756,7 @@
         <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="I23" t="s">
         <v>14</v>
@@ -1646,21 +1768,21 @@
         <v>19</v>
       </c>
       <c r="L23" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="M23" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="N23" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="O23" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1693,18 +1815,18 @@
         <v>21</v>
       </c>
       <c r="L24" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="M24" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="N24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -1728,18 +1850,18 @@
         <v>23</v>
       </c>
       <c r="L25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -1763,18 +1885,18 @@
         <v>25</v>
       </c>
       <c r="L26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="N26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -1804,15 +1926,15 @@
         <v>27</v>
       </c>
       <c r="L27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="M27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -1836,10 +1958,10 @@
         <v>29</v>
       </c>
       <c r="L28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="M28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1851,8 +1973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA569B3A-36DC-4A9C-8790-9E179146205E}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1868,7 +1990,7 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1876,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1887,10 +2009,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1899,10 +2021,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -1911,10 +2033,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1923,10 +2045,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -1935,12 +2057,199 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD14220-2B97-4004-BBA3-0B186D3485C5}">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3">
+        <v>0.01</v>
+      </c>
+      <c r="L3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="M3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4">
+        <v>-1</v>
+      </c>
+      <c r="J4">
+        <v>400</v>
+      </c>
+      <c r="K4">
+        <v>0.05</v>
+      </c>
+      <c r="L4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I5">
+        <v>50</v>
+      </c>
+      <c r="J5">
+        <v>400</v>
+      </c>
+      <c r="K5">
+        <v>0.02</v>
+      </c>
+      <c r="L5">
+        <v>2E-3</v>
+      </c>
+      <c r="M5">
+        <v>1.45</v>
+      </c>
+      <c r="N5" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support empty meta info
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDB94E7-C643-4E94-9D08-BC7F0E76014E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5256A79E-CAB3-49C8-86E2-D0BD1FA4C0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8820" yWindow="3435" windowWidth="20445" windowHeight="15345" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_map" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="103">
   <si>
     <t>id</t>
   </si>
@@ -501,9 +501,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -541,9 +541,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -576,26 +576,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -628,26 +611,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1220,7 +1186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA2FB3B-55EE-4F82-BAA9-C5D77386B2AC}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
@@ -1977,10 +1943,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA569B3A-36DC-4A9C-8790-9E179146205E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="A11:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,6 +2035,80 @@
         <v>46</v>
       </c>
       <c r="D7" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
optimize: skip zero values
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5256A79E-CAB3-49C8-86E2-D0BD1FA4C0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DE0A54-B1A7-400A-8384-E8E7D24D4E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="st_map" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="121">
   <si>
     <t>id</t>
   </si>
@@ -130,9 +130,6 @@
     <t>map</t>
   </si>
   <si>
-    <t>StData/</t>
-  </si>
-  <si>
     <t>st_map</t>
   </si>
   <si>
@@ -361,9 +358,6 @@
     <t>BulletTank</t>
   </si>
   <si>
-    <t>{"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_mapJSON","IsGenEnum":false}</t>
-  </si>
-  <si>
     <t>row:float</t>
   </si>
   <si>
@@ -425,6 +419,66 @@
   </si>
   <si>
     <t>ENUM3=67</t>
+  </si>
+  <si>
+    <t>tesbo:bool</t>
+  </si>
+  <si>
+    <t>test:float</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>ssd</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b0:float</t>
+  </si>
+  <si>
+    <t>c0:bool</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s0:string</t>
+  </si>
+  <si>
+    <t>dfdf</t>
+  </si>
+  <si>
+    <t>{"IsSkipZeroValue":false,"IsStringId":false,"IsGenItemClass":true,"JSONName":"st_mapJSON","IsGenEnum":false}</t>
   </si>
 </sst>
 </file>
@@ -787,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,21 +852,18 @@
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -823,80 +874,277 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" t="s">
+        <v>109</v>
+      </c>
+      <c r="L2" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N2" t="s">
+        <v>113</v>
+      </c>
+      <c r="O2" t="s">
+        <v>114</v>
+      </c>
+      <c r="P2" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="M3" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" t="s">
+        <v>115</v>
+      </c>
+      <c r="P3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
       <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>7.6</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+      <c r="N4" t="b">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1.5</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="b">
+        <v>0</v>
+      </c>
+      <c r="O6" t="b">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>119</v>
+      </c>
+      <c r="R6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>119</v>
+      </c>
+      <c r="R7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="P8" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -918,13 +1166,13 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -932,46 +1180,46 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" t="s">
         <v>84</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>85</v>
+      </c>
+      <c r="O2" t="s">
         <v>86</v>
-      </c>
-      <c r="N2" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1000,25 +1248,25 @@
         <v>2.5</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
       <c r="L3" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" t="s">
         <v>95</v>
       </c>
-      <c r="M3" t="s">
-        <v>97</v>
-      </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -1038,25 +1286,25 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1076,19 +1324,19 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" t="s">
-        <v>25</v>
-      </c>
       <c r="L5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1114,19 +1362,19 @@
         <v>2.4</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
         <v>26</v>
       </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
       <c r="L6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -1146,19 +1394,19 @@
         <v>1.2</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
         <v>28</v>
       </c>
-      <c r="K7" t="s">
-        <v>29</v>
-      </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
@@ -1194,13 +1442,13 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1208,52 +1456,52 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
         <v>83</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q2" t="s">
         <v>91</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>85</v>
-      </c>
-      <c r="M2" t="s">
-        <v>92</v>
-      </c>
-      <c r="N2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O2" t="s">
-        <v>87</v>
-      </c>
-      <c r="P2" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -1282,25 +1530,25 @@
         <v>2.5</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
-        <v>21</v>
-      </c>
       <c r="L3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -1320,25 +1568,25 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" t="s">
         <v>22</v>
       </c>
-      <c r="K4" t="s">
-        <v>23</v>
-      </c>
       <c r="L4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -1358,22 +1606,22 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" t="s">
-        <v>25</v>
-      </c>
       <c r="L5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="P5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -1399,22 +1647,22 @@
         <v>2.4</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s">
         <v>26</v>
       </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
       <c r="L6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="P6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1434,80 +1682,80 @@
         <v>1.2</v>
       </c>
       <c r="I7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" t="s">
         <v>28</v>
       </c>
-      <c r="K7" t="s">
-        <v>29</v>
-      </c>
       <c r="L7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" t="s">
         <v>83</v>
       </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" t="s">
-        <v>91</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
+        <v>87</v>
+      </c>
+      <c r="N12" t="s">
+        <v>84</v>
+      </c>
+      <c r="O12" t="s">
         <v>85</v>
-      </c>
-      <c r="M12" t="s">
-        <v>89</v>
-      </c>
-      <c r="N12" t="s">
-        <v>86</v>
-      </c>
-      <c r="O12" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1536,22 +1784,22 @@
         <v>2.5</v>
       </c>
       <c r="I13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" t="s">
         <v>20</v>
       </c>
-      <c r="K13" t="s">
-        <v>21</v>
-      </c>
       <c r="L13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1571,22 +1819,22 @@
         <v>3</v>
       </c>
       <c r="I14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" t="s">
         <v>22</v>
       </c>
-      <c r="K14" t="s">
-        <v>23</v>
-      </c>
       <c r="L14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1606,22 +1854,22 @@
         <v>3</v>
       </c>
       <c r="I15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" t="s">
         <v>24</v>
       </c>
-      <c r="K15" t="s">
-        <v>25</v>
-      </c>
       <c r="L15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -1647,19 +1895,19 @@
         <v>2.4</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" t="s">
         <v>26</v>
       </c>
-      <c r="K16" t="s">
-        <v>27</v>
-      </c>
       <c r="L16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -1679,82 +1927,82 @@
         <v>1.2</v>
       </c>
       <c r="I17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J17" t="s">
+        <v>27</v>
+      </c>
+      <c r="K17" t="s">
         <v>28</v>
       </c>
-      <c r="K17" t="s">
-        <v>29</v>
-      </c>
       <c r="L17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
         <v>8</v>
       </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" t="s">
+        <v>89</v>
+      </c>
+      <c r="I23" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" t="s">
+        <v>18</v>
+      </c>
+      <c r="L23" t="s">
         <v>83</v>
       </c>
-      <c r="D23" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" t="s">
-        <v>14</v>
-      </c>
-      <c r="J23" t="s">
-        <v>18</v>
-      </c>
-      <c r="K23" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
+        <v>87</v>
+      </c>
+      <c r="N23" t="s">
+        <v>84</v>
+      </c>
+      <c r="O23" t="s">
         <v>85</v>
-      </c>
-      <c r="M23" t="s">
-        <v>89</v>
-      </c>
-      <c r="N23" t="s">
-        <v>86</v>
-      </c>
-      <c r="O23" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>4</v>
@@ -1778,27 +2026,27 @@
         <v>2.5</v>
       </c>
       <c r="I24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" t="s">
+        <v>19</v>
+      </c>
+      <c r="K24" t="s">
         <v>20</v>
       </c>
-      <c r="K24" t="s">
-        <v>21</v>
-      </c>
       <c r="L24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -1813,27 +2061,27 @@
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J25" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" t="s">
         <v>22</v>
       </c>
-      <c r="K25" t="s">
-        <v>23</v>
-      </c>
       <c r="L25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26">
         <v>4</v>
@@ -1848,27 +2096,27 @@
         <v>3</v>
       </c>
       <c r="I26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J26" t="s">
+        <v>23</v>
+      </c>
+      <c r="K26" t="s">
         <v>24</v>
       </c>
-      <c r="K26" t="s">
-        <v>25</v>
-      </c>
       <c r="L26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -1889,24 +2137,24 @@
         <v>2.4</v>
       </c>
       <c r="I27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" t="s">
         <v>26</v>
       </c>
-      <c r="K27" t="s">
-        <v>27</v>
-      </c>
       <c r="L27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>4</v>
@@ -1921,19 +2169,19 @@
         <v>1.2</v>
       </c>
       <c r="I28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J28" t="s">
+        <v>27</v>
+      </c>
+      <c r="K28" t="s">
         <v>28</v>
       </c>
-      <c r="K28" t="s">
-        <v>29</v>
-      </c>
       <c r="L28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1945,8 +2193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA569B3A-36DC-4A9C-8790-9E179146205E}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="A11:C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,13 +2204,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1970,10 +2218,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1981,10 +2229,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1993,10 +2241,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -2005,10 +2253,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2017,10 +2265,10 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -2029,19 +2277,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2049,10 +2297,10 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,10 +2308,10 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2071,10 +2319,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2082,10 +2330,10 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2093,10 +2341,10 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -2104,10 +2352,10 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2127,13 +2375,13 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>49</v>
-      </c>
-      <c r="C1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -2141,43 +2389,43 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>56</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>58</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>59</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>60</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>61</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>62</v>
-      </c>
-      <c r="N2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -2185,25 +2433,25 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
         <v>64</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" t="s">
         <v>66</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>67</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>68</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>69</v>
-      </c>
-      <c r="H3" t="s">
-        <v>70</v>
       </c>
       <c r="I3">
         <v>10</v>
@@ -2221,7 +2469,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="N3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -2229,10 +2477,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
         <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
       </c>
       <c r="I4">
         <v>-1</v>
@@ -2250,7 +2498,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="N4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -2258,25 +2506,25 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" t="s">
         <v>75</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" t="s">
         <v>77</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>78</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
         <v>79</v>
-      </c>
-      <c r="G5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" t="s">
-        <v>80</v>
       </c>
       <c r="I5">
         <v>50</v>
@@ -2294,7 +2542,7 @@
         <v>1.45</v>
       </c>
       <c r="N5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: support long and double
</commit_message>
<xml_diff>
--- a/Assets/STExcelToClass/Editor/dataSample.xlsx
+++ b/Assets/STExcelToClass/Editor/dataSample.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B433C7FE-2A61-41F3-81E7-EC1C859CCC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261090B6-90E5-484D-AE85-4BF2C3AC5CB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="129">
   <si>
     <t>id</t>
   </si>
@@ -491,6 +491,18 @@
   </si>
   <si>
     <t>sdf</t>
+  </si>
+  <si>
+    <t>testLong:long</t>
+  </si>
+  <si>
+    <t>testDouble:double</t>
+  </si>
+  <si>
+    <t>testDou0:double</t>
+  </si>
+  <si>
+    <t>testDou1</t>
   </si>
 </sst>
 </file>
@@ -545,10 +557,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1165,18 +1178,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEA36E3-FED6-4ED2-8549-0F7EE0E89CF6}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="A1:P7"/>
+      <selection activeCell="Q4" sqref="A1:T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="17" max="17" width="31.28515625" customWidth="1"/>
+    <col min="18" max="18" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -1187,7 +1202,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1236,8 +1251,20 @@
       <c r="P2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" t="s">
+        <v>126</v>
+      </c>
+      <c r="S2" t="s">
+        <v>127</v>
+      </c>
+      <c r="T2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1286,8 +1313,20 @@
       <c r="P3" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q3" s="3">
+        <v>84798398239797</v>
+      </c>
+      <c r="R3">
+        <v>2.8937489237893399E+22</v>
+      </c>
+      <c r="S3">
+        <v>2.8937489237893399E+22</v>
+      </c>
+      <c r="T3">
+        <v>2.8937489237893399E+22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1327,8 +1366,20 @@
       <c r="P4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>5</v>
+      </c>
+      <c r="R4" s="3">
+        <v>84798398239797</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1362,8 +1413,17 @@
       <c r="P5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>4</v>
+      </c>
+      <c r="R5">
+        <v>5</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1403,8 +1463,14 @@
       <c r="P6" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>

</xml_diff>